<commit_message>
NumMethods: completed (really, this time) lw2
</commit_message>
<xml_diff>
--- a/Numerical methods/LW2/LW2.xlsx
+++ b/Numerical methods/LW2/LW2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24334"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\studies\Numerical methods\LW2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\studies\Numerical methods\LW2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0F2AC8E-2C42-4E44-8569-E2C9FDE7DA28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF78BF94-7200-4B09-AD3C-158636C9FD3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -29,12 +29,15 @@
         <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
+    <ext xmlns:xlwcv="http://schemas.microsoft.com/office/spreadsheetml/2024/workbookCompatibilityVersion" uri="{D14903EA-33C4-47F7-8F05-3474C54BE107}">
+      <xlwcv:version setVersion="1"/>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="14">
   <si>
     <t>-0.15012</t>
   </si>
@@ -74,14 +77,20 @@
   <si>
     <t>Метод вращений</t>
   </si>
+  <si>
+    <t>Вектор невязки</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="5">
     <numFmt numFmtId="164" formatCode="0.0000"/>
     <numFmt numFmtId="165" formatCode="0.000000"/>
+    <numFmt numFmtId="166" formatCode="0.00000"/>
+    <numFmt numFmtId="168" formatCode="#,##0.000000"/>
+    <numFmt numFmtId="169" formatCode="0.0000000"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -112,17 +121,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -403,32 +414,51 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B3:AP52"/>
+  <dimension ref="B3:CE63"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+    <sheetView tabSelected="1" topLeftCell="AF1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="CE27" sqref="CE27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="3" width="9.1796875" customWidth="1"/>
-    <col min="8" max="8" width="11.7265625" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="10.08984375" customWidth="1"/>
-    <col min="36" max="36" width="10.90625" customWidth="1"/>
-    <col min="37" max="39" width="8.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="9.140625" customWidth="1"/>
+    <col min="8" max="8" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="10.140625" customWidth="1"/>
+    <col min="36" max="36" width="10.85546875" customWidth="1"/>
+    <col min="37" max="37" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="12.28515625" customWidth="1"/>
+    <col min="40" max="40" width="12.140625" customWidth="1"/>
+    <col min="42" max="42" width="9.7109375" customWidth="1"/>
+    <col min="45" max="49" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="65" max="66" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="67" max="67" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="68" max="68" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="69" max="70" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="83" max="83" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:42" x14ac:dyDescent="0.35">
-      <c r="F3" s="3" t="s">
+    <row r="3" spans="2:83" x14ac:dyDescent="0.25">
+      <c r="F3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
-      <c r="J3" s="3"/>
-      <c r="K3" s="3"/>
-    </row>
-    <row r="4" spans="2:42" x14ac:dyDescent="0.35">
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
+      <c r="J3" s="4"/>
+      <c r="K3" s="4"/>
+      <c r="BW3" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="BX3" s="4"/>
+      <c r="BY3" s="4"/>
+      <c r="BZ3" s="4"/>
+      <c r="CA3" s="4"/>
+      <c r="CB3" s="4"/>
+    </row>
+    <row r="4" spans="2:83" x14ac:dyDescent="0.25">
       <c r="F4" s="1">
         <v>5.2403000000000004</v>
       </c>
@@ -447,8 +477,26 @@
       <c r="K4">
         <v>6.7775999999999996</v>
       </c>
-    </row>
-    <row r="5" spans="2:42" x14ac:dyDescent="0.35">
+      <c r="BW4" s="1">
+        <v>5.2403000000000004</v>
+      </c>
+      <c r="BX4" s="1">
+        <v>5.7522000000000002</v>
+      </c>
+      <c r="BY4" s="1">
+        <v>3.4759000000000002</v>
+      </c>
+      <c r="BZ4" s="1">
+        <v>-0.48749999999999999</v>
+      </c>
+      <c r="CA4" s="1">
+        <v>-1.3241000000000001</v>
+      </c>
+      <c r="CB4">
+        <v>6.7775999999999996</v>
+      </c>
+    </row>
+    <row r="5" spans="2:83" x14ac:dyDescent="0.25">
       <c r="F5" s="1">
         <v>-1.4360999999999999</v>
       </c>
@@ -467,8 +515,26 @@
       <c r="K5">
         <v>21.936199999999999</v>
       </c>
-    </row>
-    <row r="6" spans="2:42" x14ac:dyDescent="0.35">
+      <c r="BW5" s="1">
+        <v>-1.4360999999999999</v>
+      </c>
+      <c r="BX5" s="1">
+        <v>-0.22059999999999999</v>
+      </c>
+      <c r="BY5" s="1">
+        <v>-2.2722000000000002</v>
+      </c>
+      <c r="BZ5" s="1">
+        <v>9.7707999999999995</v>
+      </c>
+      <c r="CA5" s="1">
+        <v>-1.2518</v>
+      </c>
+      <c r="CB5">
+        <v>21.936199999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="2:83" x14ac:dyDescent="0.25">
       <c r="F6" s="1">
         <v>5.1886000000000001</v>
       </c>
@@ -487,8 +553,26 @@
       <c r="K6">
         <v>115.9093</v>
       </c>
-    </row>
-    <row r="7" spans="2:42" x14ac:dyDescent="0.35">
+      <c r="BW6" s="1">
+        <v>5.1886000000000001</v>
+      </c>
+      <c r="BX6" s="1">
+        <v>9.5263000000000009</v>
+      </c>
+      <c r="BY6" s="1">
+        <v>-8.0340000000000007</v>
+      </c>
+      <c r="BZ6" s="1">
+        <v>-4.2249999999999996</v>
+      </c>
+      <c r="CA6" s="1">
+        <v>-9.3440999999999992</v>
+      </c>
+      <c r="CB6">
+        <v>115.9093</v>
+      </c>
+    </row>
+    <row r="7" spans="2:83" x14ac:dyDescent="0.25">
       <c r="F7" s="1">
         <v>5.4817</v>
       </c>
@@ -507,8 +591,26 @@
       <c r="K7">
         <v>36.249299999999998</v>
       </c>
-    </row>
-    <row r="8" spans="2:42" x14ac:dyDescent="0.35">
+      <c r="BW7" s="1">
+        <v>5.4817</v>
+      </c>
+      <c r="BX7" s="1">
+        <v>-1.0106999999999999</v>
+      </c>
+      <c r="BY7" s="1">
+        <v>-6.6711</v>
+      </c>
+      <c r="BZ7" s="1">
+        <v>-4.8913000000000002</v>
+      </c>
+      <c r="CA7" s="1">
+        <v>4.4775</v>
+      </c>
+      <c r="CB7">
+        <v>36.249299999999998</v>
+      </c>
+    </row>
+    <row r="8" spans="2:83" x14ac:dyDescent="0.25">
       <c r="F8" s="1">
         <v>-2.5373000000000001</v>
       </c>
@@ -527,66 +629,84 @@
       <c r="K8">
         <v>47.121200000000002</v>
       </c>
-    </row>
-    <row r="10" spans="2:42" x14ac:dyDescent="0.35">
-      <c r="B10" s="3" t="s">
+      <c r="BW8" s="1">
+        <v>-2.5373000000000001</v>
+      </c>
+      <c r="BX8" s="1">
+        <v>2.5573000000000001</v>
+      </c>
+      <c r="BY8" s="1">
+        <v>-6.9600999999999997</v>
+      </c>
+      <c r="BZ8" s="1">
+        <v>9.6417000000000002</v>
+      </c>
+      <c r="CA8" s="1">
+        <v>-2.7947000000000002</v>
+      </c>
+      <c r="CB8">
+        <v>47.121200000000002</v>
+      </c>
+    </row>
+    <row r="10" spans="2:83" x14ac:dyDescent="0.25">
+      <c r="B10" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
-      <c r="I10" s="3"/>
-      <c r="J10" s="3"/>
-      <c r="K10" s="3"/>
-      <c r="L10" s="3"/>
-      <c r="M10" s="3"/>
-      <c r="N10" s="3"/>
-      <c r="O10" s="3"/>
-      <c r="T10" s="3" t="s">
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
+      <c r="I10" s="4"/>
+      <c r="J10" s="4"/>
+      <c r="K10" s="4"/>
+      <c r="L10" s="4"/>
+      <c r="M10" s="4"/>
+      <c r="N10" s="4"/>
+      <c r="O10" s="4"/>
+      <c r="T10" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="U10" s="3"/>
-      <c r="V10" s="3"/>
-      <c r="W10" s="3"/>
-      <c r="X10" s="3"/>
-      <c r="Y10" s="3"/>
-      <c r="AI10" s="3" t="s">
+      <c r="U10" s="4"/>
+      <c r="V10" s="4"/>
+      <c r="W10" s="4"/>
+      <c r="X10" s="4"/>
+      <c r="Y10" s="4"/>
+      <c r="AI10" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="AJ10" s="3"/>
-      <c r="AK10" s="3"/>
-      <c r="AL10" s="3"/>
-      <c r="AM10" s="3"/>
-      <c r="AN10" s="3"/>
-    </row>
-    <row r="11" spans="2:42" x14ac:dyDescent="0.35">
-      <c r="B11" s="3" t="s">
+      <c r="AJ10" s="4"/>
+      <c r="AK10" s="4"/>
+      <c r="AL10" s="4"/>
+      <c r="AM10" s="4"/>
+      <c r="AN10" s="4"/>
+    </row>
+    <row r="11" spans="2:83" x14ac:dyDescent="0.25">
+      <c r="B11" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
-      <c r="J11" s="3" t="s">
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
+      <c r="J11" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="K11" s="3"/>
-      <c r="L11" s="3"/>
-      <c r="M11" s="3"/>
-      <c r="N11" s="3"/>
-      <c r="O11" s="3"/>
-      <c r="AA11" s="3" t="s">
+      <c r="K11" s="4"/>
+      <c r="L11" s="4"/>
+      <c r="M11" s="4"/>
+      <c r="N11" s="4"/>
+      <c r="O11" s="4"/>
+      <c r="AA11" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="AB11" s="3"/>
-      <c r="AC11" s="3" t="s">
+      <c r="AB11" s="4"/>
+      <c r="AC11" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="AD11" s="3"/>
+      <c r="AD11" s="4"/>
       <c r="AI11" s="1">
         <v>5.2403000000000004</v>
       </c>
@@ -609,8 +729,96 @@
         <f>SQRT(AI11^2 + AI12^2)</f>
         <v>5.4335188690203333</v>
       </c>
-    </row>
-    <row r="12" spans="2:42" x14ac:dyDescent="0.35">
+      <c r="AS11">
+        <v>9.6401199999999996</v>
+      </c>
+      <c r="AT11">
+        <v>7.0392799999999998</v>
+      </c>
+      <c r="AU11">
+        <v>-4.05769</v>
+      </c>
+      <c r="AV11">
+        <v>-9.3136899999999994</v>
+      </c>
+      <c r="AW11">
+        <v>-2.2809400000000002</v>
+      </c>
+      <c r="AX11">
+        <v>71.012680000000003</v>
+      </c>
+      <c r="AZ11">
+        <f>SQRT(AT12^2 + AT13^2)</f>
+        <v>3.2891099686389325</v>
+      </c>
+      <c r="BC11">
+        <v>9.6401199999999996</v>
+      </c>
+      <c r="BD11">
+        <v>7.0392799999999998</v>
+      </c>
+      <c r="BE11">
+        <v>-4.05769</v>
+      </c>
+      <c r="BF11">
+        <v>-9.3136899999999994</v>
+      </c>
+      <c r="BG11">
+        <v>-2.2809400000000002</v>
+      </c>
+      <c r="BH11">
+        <v>71.012680000000003</v>
+      </c>
+      <c r="BJ11">
+        <f>SQRT(BE13^2 +BE14^2)</f>
+        <v>9.4350803312425473</v>
+      </c>
+      <c r="BM11" s="7">
+        <v>9.6401199999999996</v>
+      </c>
+      <c r="BN11" s="7">
+        <v>7.0392799999999998</v>
+      </c>
+      <c r="BO11" s="7">
+        <v>-4.05769</v>
+      </c>
+      <c r="BP11" s="7">
+        <v>-9.3136899999999994</v>
+      </c>
+      <c r="BQ11" s="7">
+        <v>-2.2809400000000002</v>
+      </c>
+      <c r="BR11" s="7">
+        <v>71.012680000000003</v>
+      </c>
+      <c r="BT11">
+        <f>SQRT(BP14^2 +BP15^2)</f>
+        <v>10.125876483450705</v>
+      </c>
+      <c r="BW11">
+        <v>9.6401199999999996</v>
+      </c>
+      <c r="BX11">
+        <v>7.0392799999999998</v>
+      </c>
+      <c r="BY11">
+        <v>-4.05769</v>
+      </c>
+      <c r="BZ11">
+        <v>-9.3136899999999994</v>
+      </c>
+      <c r="CA11">
+        <v>-2.2809400000000002</v>
+      </c>
+      <c r="CB11">
+        <v>71.012680000000003</v>
+      </c>
+      <c r="CD11" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="CE11" s="4"/>
+    </row>
+    <row r="12" spans="2:83" x14ac:dyDescent="0.25">
       <c r="B12" s="1">
         <v>5.2403000000000004</v>
       </c>
@@ -697,8 +905,87 @@
       <c r="AN12">
         <v>21.936199999999999</v>
       </c>
-    </row>
-    <row r="13" spans="2:42" x14ac:dyDescent="0.35">
+      <c r="AS12">
+        <v>0</v>
+      </c>
+      <c r="AT12">
+        <v>1.3075699999999999</v>
+      </c>
+      <c r="AU12">
+        <v>-1.2726999999999999</v>
+      </c>
+      <c r="AV12">
+        <v>9.2944899999999997</v>
+      </c>
+      <c r="AW12">
+        <v>-1.55725</v>
+      </c>
+      <c r="AX12">
+        <v>22.947469999999999</v>
+      </c>
+      <c r="BC12">
+        <v>0</v>
+      </c>
+      <c r="BD12">
+        <v>9.0496999999999996</v>
+      </c>
+      <c r="BE12">
+        <v>-4.2578800000000001</v>
+      </c>
+      <c r="BF12">
+        <v>5.5198999999999998</v>
+      </c>
+      <c r="BG12">
+        <v>-10.16292</v>
+      </c>
+      <c r="BH12">
+        <v>79.817580000000007</v>
+      </c>
+      <c r="BM12" s="7">
+        <v>0</v>
+      </c>
+      <c r="BN12" s="7">
+        <v>9.0496999999999996</v>
+      </c>
+      <c r="BO12" s="7">
+        <v>-4.2578800000000001</v>
+      </c>
+      <c r="BP12" s="7">
+        <v>5.5198999999999998</v>
+      </c>
+      <c r="BQ12" s="7">
+        <v>-10.16292</v>
+      </c>
+      <c r="BR12" s="7">
+        <v>79.817580000000007</v>
+      </c>
+      <c r="BW12">
+        <v>0</v>
+      </c>
+      <c r="BX12">
+        <v>9.0496999999999996</v>
+      </c>
+      <c r="BY12">
+        <v>-4.2578800000000001</v>
+      </c>
+      <c r="BZ12">
+        <v>5.5198999999999998</v>
+      </c>
+      <c r="CA12">
+        <v>-10.16292</v>
+      </c>
+      <c r="CB12">
+        <v>79.817580000000007</v>
+      </c>
+      <c r="CD12" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="CE12">
+        <f>CB4 - BW4*$CB$41 - BX4*$CB$42 - BY4*$CB$43 - BZ4*$CB$44 - CA4*$CB$45</f>
+        <v>-1.1560000000798709E-5</v>
+      </c>
+    </row>
+    <row r="13" spans="2:83" x14ac:dyDescent="0.25">
       <c r="B13" s="1">
         <v>-1.4360999999999999</v>
       </c>
@@ -775,8 +1062,84 @@
       <c r="AN13">
         <v>115.9093</v>
       </c>
-    </row>
-    <row r="14" spans="2:42" x14ac:dyDescent="0.35">
+      <c r="AS13">
+        <v>0</v>
+      </c>
+      <c r="AT13">
+        <v>3.01803</v>
+      </c>
+      <c r="AU13">
+        <v>-8.5402699999999996</v>
+      </c>
+      <c r="AV13">
+        <v>-0.94740000000000002</v>
+      </c>
+      <c r="AW13">
+        <v>-6.1044</v>
+      </c>
+      <c r="AX13">
+        <v>83.317719999999994</v>
+      </c>
+      <c r="BC13">
+        <v>0</v>
+      </c>
+      <c r="BD13">
+        <v>0</v>
+      </c>
+      <c r="BE13">
+        <v>-2.2273299999999998</v>
+      </c>
+      <c r="BF13">
+        <v>-8.9050999999999991</v>
+      </c>
+      <c r="BG13">
+        <v>-0.99787000000000003</v>
+      </c>
+      <c r="BH13">
+        <v>12.066330000000001</v>
+      </c>
+      <c r="BM13" s="7">
+        <v>0</v>
+      </c>
+      <c r="BN13" s="7">
+        <v>0</v>
+      </c>
+      <c r="BO13" s="7">
+        <v>11.838179999999999</v>
+      </c>
+      <c r="BP13" s="7">
+        <v>-3.2705799999999998</v>
+      </c>
+      <c r="BQ13" s="7">
+        <v>0.87565999999999999</v>
+      </c>
+      <c r="BR13" s="7">
+        <v>-75.965549999999993</v>
+      </c>
+      <c r="BW13">
+        <v>0</v>
+      </c>
+      <c r="BX13">
+        <v>0</v>
+      </c>
+      <c r="BY13">
+        <v>11.838179999999999</v>
+      </c>
+      <c r="BZ13">
+        <v>-3.2705799999999998</v>
+      </c>
+      <c r="CA13">
+        <v>0.87565999999999999</v>
+      </c>
+      <c r="CB13">
+        <v>-75.965549999999993</v>
+      </c>
+      <c r="CE13">
+        <f t="shared" ref="CE13:CE16" si="1">CB5 - BW5*$CB$41 - BX5*$CB$42 - BY5*$CB$43 - BZ5*$CB$44 - CA5*$CB$45</f>
+        <v>-3.1671000002120309E-5</v>
+      </c>
+    </row>
+    <row r="14" spans="2:83" x14ac:dyDescent="0.25">
       <c r="B14" s="1">
         <v>5.1886000000000001</v>
       </c>
@@ -853,8 +1216,84 @@
       <c r="AN14">
         <v>36.249299999999998</v>
       </c>
-    </row>
-    <row r="15" spans="2:42" x14ac:dyDescent="0.35">
+      <c r="AS14">
+        <v>0</v>
+      </c>
+      <c r="AT14">
+        <v>-7.0839699999999999</v>
+      </c>
+      <c r="AU14">
+        <v>-3.8037800000000002</v>
+      </c>
+      <c r="AV14">
+        <v>-0.93022000000000005</v>
+      </c>
+      <c r="AW14">
+        <v>7.82402</v>
+      </c>
+      <c r="AX14">
+        <v>-18.214089999999999</v>
+      </c>
+      <c r="BC14">
+        <v>0</v>
+      </c>
+      <c r="BD14">
+        <v>0</v>
+      </c>
+      <c r="BE14">
+        <v>-9.1684099999999997</v>
+      </c>
+      <c r="BF14">
+        <v>2.1711399999999998</v>
+      </c>
+      <c r="BG14">
+        <v>-2.34701</v>
+      </c>
+      <c r="BH14">
+        <v>69.945099999999996</v>
+      </c>
+      <c r="BM14" s="7">
+        <v>0</v>
+      </c>
+      <c r="BN14" s="7">
+        <v>0</v>
+      </c>
+      <c r="BO14" s="7">
+        <v>0</v>
+      </c>
+      <c r="BP14" s="7">
+        <v>-9.1659500000000005</v>
+      </c>
+      <c r="BQ14" s="7">
+        <v>-0.41560999999999998</v>
+      </c>
+      <c r="BR14" s="7">
+        <v>-4.7865799999999998</v>
+      </c>
+      <c r="BW14">
+        <v>0</v>
+      </c>
+      <c r="BX14">
+        <v>0</v>
+      </c>
+      <c r="BY14">
+        <v>0</v>
+      </c>
+      <c r="BZ14">
+        <v>10.12588</v>
+      </c>
+      <c r="CA14">
+        <v>1.65568</v>
+      </c>
+      <c r="CB14">
+        <v>-2.8949099999999999</v>
+      </c>
+      <c r="CE14">
+        <f t="shared" si="1"/>
+        <v>-3.1078999988665146E-5</v>
+      </c>
+    </row>
+    <row r="15" spans="2:83" x14ac:dyDescent="0.25">
       <c r="B15" s="1">
         <v>5.4817</v>
       </c>
@@ -931,8 +1370,84 @@
       <c r="AN15">
         <v>47.121200000000002</v>
       </c>
-    </row>
-    <row r="16" spans="2:42" x14ac:dyDescent="0.35">
+      <c r="AS15">
+        <v>0</v>
+      </c>
+      <c r="AT15">
+        <v>4.5712299999999999</v>
+      </c>
+      <c r="AU15">
+        <v>-8.3215000000000003</v>
+      </c>
+      <c r="AV15">
+        <v>7.4531099999999997</v>
+      </c>
+      <c r="AW15">
+        <v>-3.5191300000000001</v>
+      </c>
+      <c r="AX15">
+        <v>68.217169999999996</v>
+      </c>
+      <c r="BC15">
+        <v>0</v>
+      </c>
+      <c r="BD15">
+        <v>0</v>
+      </c>
+      <c r="BE15">
+        <v>-7.1499499999999996</v>
+      </c>
+      <c r="BF15">
+        <v>5.4051200000000001</v>
+      </c>
+      <c r="BG15">
+        <v>1.8706</v>
+      </c>
+      <c r="BH15">
+        <v>32.326540000000001</v>
+      </c>
+      <c r="BM15" s="7">
+        <v>0</v>
+      </c>
+      <c r="BN15" s="7">
+        <v>0</v>
+      </c>
+      <c r="BO15" s="7">
+        <v>0</v>
+      </c>
+      <c r="BP15" s="7">
+        <v>4.3033400000000004</v>
+      </c>
+      <c r="BQ15" s="7">
+        <v>3.0106199999999999</v>
+      </c>
+      <c r="BR15" s="7">
+        <v>-17.00704</v>
+      </c>
+      <c r="BW15">
+        <v>0</v>
+      </c>
+      <c r="BX15">
+        <v>0</v>
+      </c>
+      <c r="BY15">
+        <v>0</v>
+      </c>
+      <c r="BZ15">
+        <v>0</v>
+      </c>
+      <c r="CA15">
+        <v>-2.5485899999999999</v>
+      </c>
+      <c r="CB15">
+        <v>17.429010000000002</v>
+      </c>
+      <c r="CE15">
+        <f t="shared" si="1"/>
+        <v>6.664600000405585E-5</v>
+      </c>
+    </row>
+    <row r="16" spans="2:83" x14ac:dyDescent="0.25">
       <c r="B16" s="1">
         <v>-2.5373000000000001</v>
       </c>
@@ -991,27 +1506,94 @@
         <f t="shared" si="0"/>
         <v>7.0689299999315836E-4</v>
       </c>
-    </row>
-    <row r="17" spans="2:40" x14ac:dyDescent="0.35">
-      <c r="AI17" s="4">
+      <c r="CE16">
+        <f t="shared" si="1"/>
+        <v>1.3780000003293935E-6</v>
+      </c>
+    </row>
+    <row r="17" spans="2:83" x14ac:dyDescent="0.25">
+      <c r="AI17" s="3">
         <f>AI11 / AP11</f>
         <v>0.96443945927527985</v>
       </c>
-      <c r="AJ17" s="4">
+      <c r="AJ17" s="3">
         <f>AI12 / AP11</f>
         <v>-0.26430385807400897</v>
       </c>
-      <c r="AK17" s="4">
-        <v>0</v>
-      </c>
-      <c r="AL17" s="4">
-        <v>0</v>
-      </c>
-      <c r="AM17" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="2:40" x14ac:dyDescent="0.35">
+      <c r="AK17" s="3">
+        <v>0</v>
+      </c>
+      <c r="AL17" s="3">
+        <v>0</v>
+      </c>
+      <c r="AM17" s="3">
+        <v>0</v>
+      </c>
+      <c r="AS17" s="3">
+        <v>1</v>
+      </c>
+      <c r="AT17" s="3">
+        <v>0</v>
+      </c>
+      <c r="AU17" s="3">
+        <v>0</v>
+      </c>
+      <c r="AV17" s="3">
+        <v>0</v>
+      </c>
+      <c r="AW17" s="3">
+        <v>0</v>
+      </c>
+      <c r="BC17" s="6">
+        <v>1</v>
+      </c>
+      <c r="BD17" s="6">
+        <v>0</v>
+      </c>
+      <c r="BE17" s="6">
+        <v>0</v>
+      </c>
+      <c r="BF17" s="6">
+        <v>0</v>
+      </c>
+      <c r="BG17" s="6">
+        <v>0</v>
+      </c>
+      <c r="BM17" s="7">
+        <v>1</v>
+      </c>
+      <c r="BN17" s="7">
+        <v>0</v>
+      </c>
+      <c r="BO17" s="7">
+        <v>0</v>
+      </c>
+      <c r="BP17" s="7">
+        <v>0</v>
+      </c>
+      <c r="BQ17" s="7">
+        <v>0</v>
+      </c>
+      <c r="BW17">
+        <v>9.6401199999999996</v>
+      </c>
+      <c r="BX17">
+        <v>7.0392799999999998</v>
+      </c>
+      <c r="BY17">
+        <v>-4.05769</v>
+      </c>
+      <c r="BZ17">
+        <v>-9.3136899999999994</v>
+      </c>
+      <c r="CA17">
+        <v>0</v>
+      </c>
+      <c r="CB17">
+        <v>55.41404</v>
+      </c>
+    </row>
+    <row r="18" spans="2:83" x14ac:dyDescent="0.25">
       <c r="B18">
         <v>1</v>
       </c>
@@ -1066,25 +1648,94 @@
       <c r="Y18">
         <v>-16.147849999999998</v>
       </c>
-      <c r="AI18" s="4">
+      <c r="AI18" s="3">
         <f>-AI12/AP11</f>
         <v>0.26430385807400897</v>
       </c>
-      <c r="AJ18" s="4">
+      <c r="AJ18" s="3">
         <f>AI11 / AP11</f>
         <v>0.96443945927527985</v>
       </c>
-      <c r="AK18" s="4">
-        <v>0</v>
-      </c>
-      <c r="AL18" s="4">
-        <v>0</v>
-      </c>
-      <c r="AM18" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="2:40" x14ac:dyDescent="0.35">
+      <c r="AK18" s="3">
+        <v>0</v>
+      </c>
+      <c r="AL18" s="3">
+        <v>0</v>
+      </c>
+      <c r="AM18" s="3">
+        <v>0</v>
+      </c>
+      <c r="AS18" s="3">
+        <v>0</v>
+      </c>
+      <c r="AT18" s="3">
+        <f>AT12/AZ11</f>
+        <v>0.39754523639143807</v>
+      </c>
+      <c r="AU18" s="3">
+        <f>AT13/AZ11</f>
+        <v>0.91758257667769372</v>
+      </c>
+      <c r="AV18" s="3">
+        <v>0</v>
+      </c>
+      <c r="AW18" s="3">
+        <v>0</v>
+      </c>
+      <c r="BC18" s="6">
+        <v>0</v>
+      </c>
+      <c r="BD18" s="6">
+        <v>1</v>
+      </c>
+      <c r="BE18" s="6">
+        <v>0</v>
+      </c>
+      <c r="BF18" s="6">
+        <v>0</v>
+      </c>
+      <c r="BG18" s="6">
+        <v>0</v>
+      </c>
+      <c r="BM18" s="7">
+        <v>0</v>
+      </c>
+      <c r="BN18" s="7">
+        <v>1</v>
+      </c>
+      <c r="BO18" s="7">
+        <v>0</v>
+      </c>
+      <c r="BP18" s="7">
+        <v>0</v>
+      </c>
+      <c r="BQ18" s="7">
+        <v>0</v>
+      </c>
+      <c r="BW18">
+        <v>0</v>
+      </c>
+      <c r="BX18">
+        <v>9.0496999999999996</v>
+      </c>
+      <c r="BY18">
+        <v>-4.2578800000000001</v>
+      </c>
+      <c r="BZ18">
+        <v>5.5198999999999998</v>
+      </c>
+      <c r="CA18">
+        <v>0</v>
+      </c>
+      <c r="CB18">
+        <v>10.316520000000001</v>
+      </c>
+      <c r="CD18" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="CE18" s="4"/>
+    </row>
+    <row r="19" spans="2:83" x14ac:dyDescent="0.25">
       <c r="B19">
         <v>0</v>
       </c>
@@ -1139,23 +1790,97 @@
       <c r="Y19">
         <v>2.2450800000000002</v>
       </c>
-      <c r="AI19" s="4">
-        <v>0</v>
-      </c>
-      <c r="AJ19" s="4">
-        <v>0</v>
-      </c>
-      <c r="AK19" s="4">
-        <v>1</v>
-      </c>
-      <c r="AL19" s="4">
-        <v>0</v>
-      </c>
-      <c r="AM19" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="2:40" x14ac:dyDescent="0.35">
+      <c r="AI19" s="3">
+        <v>0</v>
+      </c>
+      <c r="AJ19" s="3">
+        <v>0</v>
+      </c>
+      <c r="AK19" s="3">
+        <v>1</v>
+      </c>
+      <c r="AL19" s="3">
+        <v>0</v>
+      </c>
+      <c r="AM19" s="3">
+        <v>0</v>
+      </c>
+      <c r="AS19" s="3">
+        <v>0</v>
+      </c>
+      <c r="AT19" s="3">
+        <f>-AT13/AZ11</f>
+        <v>-0.91758257667769372</v>
+      </c>
+      <c r="AU19" s="3">
+        <f>AT12/AZ11</f>
+        <v>0.39754523639143807</v>
+      </c>
+      <c r="AV19" s="3">
+        <v>0</v>
+      </c>
+      <c r="AW19" s="3">
+        <v>0</v>
+      </c>
+      <c r="BC19" s="6">
+        <v>0</v>
+      </c>
+      <c r="BD19" s="6">
+        <v>0</v>
+      </c>
+      <c r="BE19" s="6">
+        <f>BE13/BJ11</f>
+        <v>-0.23606900225582636</v>
+      </c>
+      <c r="BF19" s="6">
+        <f>BE14/BJ11</f>
+        <v>-0.97173629456449695</v>
+      </c>
+      <c r="BG19" s="6">
+        <v>0</v>
+      </c>
+      <c r="BM19" s="7">
+        <v>0</v>
+      </c>
+      <c r="BN19" s="7">
+        <v>0</v>
+      </c>
+      <c r="BO19" s="7">
+        <v>1</v>
+      </c>
+      <c r="BP19" s="7">
+        <v>0</v>
+      </c>
+      <c r="BQ19" s="7">
+        <v>0</v>
+      </c>
+      <c r="BW19">
+        <v>0</v>
+      </c>
+      <c r="BX19">
+        <v>0</v>
+      </c>
+      <c r="BY19">
+        <v>11.838179999999999</v>
+      </c>
+      <c r="BZ19">
+        <v>-3.2705799999999998</v>
+      </c>
+      <c r="CA19">
+        <v>0</v>
+      </c>
+      <c r="CB19">
+        <v>-69.977180000000004</v>
+      </c>
+      <c r="CD19" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="CE19">
+        <f>SQRT(CE12^2 +CE13^2 +CE14^2 +CE15^2 +CE16^2)</f>
+        <v>8.0908456183453038E-5</v>
+      </c>
+    </row>
+    <row r="20" spans="2:83" x14ac:dyDescent="0.25">
       <c r="B20">
         <v>0</v>
       </c>
@@ -1210,23 +1935,90 @@
       <c r="Y20">
         <v>-29.67923</v>
       </c>
-      <c r="AI20" s="4">
-        <v>0</v>
-      </c>
-      <c r="AJ20" s="4">
-        <v>0</v>
-      </c>
-      <c r="AK20" s="4">
-        <v>0</v>
-      </c>
-      <c r="AL20" s="4">
-        <v>1</v>
-      </c>
-      <c r="AM20" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="2:40" x14ac:dyDescent="0.35">
+      <c r="AI20" s="3">
+        <v>0</v>
+      </c>
+      <c r="AJ20" s="3">
+        <v>0</v>
+      </c>
+      <c r="AK20" s="3">
+        <v>0</v>
+      </c>
+      <c r="AL20" s="3">
+        <v>1</v>
+      </c>
+      <c r="AM20" s="3">
+        <v>0</v>
+      </c>
+      <c r="AS20" s="3">
+        <v>0</v>
+      </c>
+      <c r="AT20" s="3">
+        <v>0</v>
+      </c>
+      <c r="AU20" s="3">
+        <v>0</v>
+      </c>
+      <c r="AV20" s="3">
+        <v>1</v>
+      </c>
+      <c r="AW20" s="3">
+        <v>0</v>
+      </c>
+      <c r="BC20" s="6">
+        <v>0</v>
+      </c>
+      <c r="BD20" s="6">
+        <v>0</v>
+      </c>
+      <c r="BE20" s="6">
+        <f>-BE14/BJ11</f>
+        <v>0.97173629456449695</v>
+      </c>
+      <c r="BF20" s="6">
+        <f>BE13/BJ11</f>
+        <v>-0.23606900225582636</v>
+      </c>
+      <c r="BG20" s="6">
+        <v>0</v>
+      </c>
+      <c r="BM20" s="7">
+        <v>0</v>
+      </c>
+      <c r="BN20" s="7">
+        <v>0</v>
+      </c>
+      <c r="BO20" s="7">
+        <v>0</v>
+      </c>
+      <c r="BP20" s="7">
+        <f>BP14/BT11</f>
+        <v>-0.90520065250454451</v>
+      </c>
+      <c r="BQ20" s="7">
+        <f>BP15/BT11</f>
+        <v>0.42498444525105489</v>
+      </c>
+      <c r="BW20">
+        <v>0</v>
+      </c>
+      <c r="BX20">
+        <v>0</v>
+      </c>
+      <c r="BY20">
+        <v>0</v>
+      </c>
+      <c r="BZ20">
+        <v>10.12588</v>
+      </c>
+      <c r="CA20">
+        <v>0</v>
+      </c>
+      <c r="CB20">
+        <v>8.4277700000000006</v>
+      </c>
+    </row>
+    <row r="21" spans="2:83" x14ac:dyDescent="0.25">
       <c r="B21">
         <v>0</v>
       </c>
@@ -1281,23 +2073,88 @@
       <c r="Y21">
         <v>-9.6560500000000005</v>
       </c>
-      <c r="AI21" s="4">
-        <v>0</v>
-      </c>
-      <c r="AJ21" s="4">
-        <v>0</v>
-      </c>
-      <c r="AK21" s="4">
-        <v>0</v>
-      </c>
-      <c r="AL21" s="4">
-        <v>0</v>
-      </c>
-      <c r="AM21" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="2:40" x14ac:dyDescent="0.35">
+      <c r="AI21" s="3">
+        <v>0</v>
+      </c>
+      <c r="AJ21" s="3">
+        <v>0</v>
+      </c>
+      <c r="AK21" s="3">
+        <v>0</v>
+      </c>
+      <c r="AL21" s="3">
+        <v>0</v>
+      </c>
+      <c r="AM21" s="3">
+        <v>1</v>
+      </c>
+      <c r="AS21" s="3">
+        <v>0</v>
+      </c>
+      <c r="AT21" s="3">
+        <v>0</v>
+      </c>
+      <c r="AU21" s="3">
+        <v>0</v>
+      </c>
+      <c r="AV21" s="3">
+        <v>0</v>
+      </c>
+      <c r="AW21" s="3">
+        <v>1</v>
+      </c>
+      <c r="BC21" s="6">
+        <v>0</v>
+      </c>
+      <c r="BD21" s="6">
+        <v>0</v>
+      </c>
+      <c r="BE21" s="6">
+        <v>0</v>
+      </c>
+      <c r="BF21" s="6">
+        <v>0</v>
+      </c>
+      <c r="BG21" s="6">
+        <v>1</v>
+      </c>
+      <c r="BM21" s="7">
+        <v>0</v>
+      </c>
+      <c r="BN21" s="7">
+        <v>0</v>
+      </c>
+      <c r="BO21" s="7">
+        <v>0</v>
+      </c>
+      <c r="BP21" s="7">
+        <f>-BP15/BT11</f>
+        <v>-0.42498444525105489</v>
+      </c>
+      <c r="BQ21" s="7">
+        <f>BP14/BT11</f>
+        <v>-0.90520065250454451</v>
+      </c>
+      <c r="BW21">
+        <v>0</v>
+      </c>
+      <c r="BX21">
+        <v>0</v>
+      </c>
+      <c r="BY21">
+        <v>0</v>
+      </c>
+      <c r="BZ21">
+        <v>0</v>
+      </c>
+      <c r="CA21">
+        <v>1</v>
+      </c>
+      <c r="CB21">
+        <v>-6.8386899999999997</v>
+      </c>
+    </row>
+    <row r="22" spans="2:83" x14ac:dyDescent="0.25">
       <c r="B22">
         <v>0</v>
       </c>
@@ -1353,27 +2210,111 @@
         <v>2.64215</v>
       </c>
     </row>
-    <row r="23" spans="2:40" x14ac:dyDescent="0.35">
-      <c r="AI23">
+    <row r="23" spans="2:83" x14ac:dyDescent="0.25">
+      <c r="AI23" s="5">
         <v>5.4335199999999997</v>
       </c>
-      <c r="AJ23">
+      <c r="AJ23" s="5">
         <v>5.60595</v>
       </c>
-      <c r="AK23">
+      <c r="AK23" s="5">
         <v>3.9528500000000002</v>
       </c>
-      <c r="AL23">
+      <c r="AL23" s="5">
         <v>-3.0526300000000002</v>
       </c>
-      <c r="AM23">
+      <c r="AM23" s="5">
         <v>-0.94616</v>
       </c>
-      <c r="AN23">
+      <c r="AN23" s="5">
         <v>0.73875999999999997</v>
       </c>
-    </row>
-    <row r="24" spans="2:40" x14ac:dyDescent="0.35">
+      <c r="AP23">
+        <f>SQRT(AI23^2 + AI25^2)</f>
+        <v>7.512969422964531</v>
+      </c>
+      <c r="AS23" s="3">
+        <v>9.6401199999999996</v>
+      </c>
+      <c r="AT23" s="3">
+        <v>7.0392799999999998</v>
+      </c>
+      <c r="AU23" s="3">
+        <v>-4.05769</v>
+      </c>
+      <c r="AV23" s="3">
+        <v>-9.3136899999999994</v>
+      </c>
+      <c r="AW23" s="3">
+        <v>-2.2809400000000002</v>
+      </c>
+      <c r="AX23" s="3">
+        <v>71.012680000000003</v>
+      </c>
+      <c r="AZ23">
+        <f>SQRT(AT24^2 + AT26^2)</f>
+        <v>7.8103057272426923</v>
+      </c>
+      <c r="BC23">
+        <v>9.6401199999999996</v>
+      </c>
+      <c r="BD23">
+        <v>7.0392799999999998</v>
+      </c>
+      <c r="BE23">
+        <v>-4.05769</v>
+      </c>
+      <c r="BF23">
+        <v>-9.3136899999999994</v>
+      </c>
+      <c r="BG23">
+        <v>-2.2809400000000002</v>
+      </c>
+      <c r="BH23">
+        <v>71.012680000000003</v>
+      </c>
+      <c r="BJ23">
+        <f>SQRT(BE25^2 +BE27^2)</f>
+        <v>11.838180586935646</v>
+      </c>
+      <c r="BM23">
+        <v>9.6401199999999996</v>
+      </c>
+      <c r="BN23">
+        <v>7.0392799999999998</v>
+      </c>
+      <c r="BO23">
+        <v>-4.05769</v>
+      </c>
+      <c r="BP23">
+        <v>-9.3136899999999994</v>
+      </c>
+      <c r="BQ23">
+        <v>-2.2809400000000002</v>
+      </c>
+      <c r="BR23">
+        <v>71.012680000000003</v>
+      </c>
+      <c r="BW23">
+        <v>9.6401199999999996</v>
+      </c>
+      <c r="BX23">
+        <v>7.0392799999999998</v>
+      </c>
+      <c r="BY23">
+        <v>-4.05769</v>
+      </c>
+      <c r="BZ23">
+        <v>0</v>
+      </c>
+      <c r="CA23">
+        <v>0</v>
+      </c>
+      <c r="CB23">
+        <v>63.165819999999997</v>
+      </c>
+    </row>
+    <row r="24" spans="2:83" x14ac:dyDescent="0.25">
       <c r="B24">
         <v>1</v>
       </c>
@@ -1428,26 +2369,98 @@
       <c r="Y24">
         <v>1.3711599999999999</v>
       </c>
-      <c r="AI24">
-        <v>0</v>
-      </c>
-      <c r="AJ24">
+      <c r="AI24" s="5">
+        <v>0</v>
+      </c>
+      <c r="AJ24" s="5">
         <v>1.3075699999999999</v>
       </c>
-      <c r="AK24">
+      <c r="AK24" s="5">
         <v>-1.2726999999999999</v>
       </c>
-      <c r="AL24">
+      <c r="AL24" s="5">
         <v>9.2944899999999997</v>
       </c>
-      <c r="AM24">
+      <c r="AM24" s="5">
         <v>-1.55725</v>
       </c>
-      <c r="AN24">
+      <c r="AN24" s="5">
         <v>22.947469999999999</v>
       </c>
-    </row>
-    <row r="25" spans="2:40" x14ac:dyDescent="0.35">
+      <c r="AS24" s="3">
+        <v>0</v>
+      </c>
+      <c r="AT24" s="3">
+        <v>3.28911</v>
+      </c>
+      <c r="AU24" s="3">
+        <v>-8.3423599999999993</v>
+      </c>
+      <c r="AV24" s="3">
+        <v>2.8256600000000001</v>
+      </c>
+      <c r="AW24" s="3">
+        <v>-6.22037</v>
+      </c>
+      <c r="AX24" s="3">
+        <v>85.573580000000007</v>
+      </c>
+      <c r="BC24">
+        <v>0</v>
+      </c>
+      <c r="BD24">
+        <v>9.0496999999999996</v>
+      </c>
+      <c r="BE24">
+        <v>-4.2578800000000001</v>
+      </c>
+      <c r="BF24">
+        <v>5.5198999999999998</v>
+      </c>
+      <c r="BG24">
+        <v>-10.16292</v>
+      </c>
+      <c r="BH24">
+        <v>79.817580000000007</v>
+      </c>
+      <c r="BM24">
+        <v>0</v>
+      </c>
+      <c r="BN24">
+        <v>9.0496999999999996</v>
+      </c>
+      <c r="BO24">
+        <v>-4.2578800000000001</v>
+      </c>
+      <c r="BP24">
+        <v>5.5198999999999998</v>
+      </c>
+      <c r="BQ24">
+        <v>-10.16292</v>
+      </c>
+      <c r="BR24">
+        <v>79.817580000000007</v>
+      </c>
+      <c r="BW24">
+        <v>0</v>
+      </c>
+      <c r="BX24">
+        <v>9.0496999999999996</v>
+      </c>
+      <c r="BY24">
+        <v>-4.2578800000000001</v>
+      </c>
+      <c r="BZ24">
+        <v>0</v>
+      </c>
+      <c r="CA24">
+        <v>0</v>
+      </c>
+      <c r="CB24">
+        <v>5.7223100000000002</v>
+      </c>
+    </row>
+    <row r="25" spans="2:83" x14ac:dyDescent="0.25">
       <c r="B25">
         <v>0</v>
       </c>
@@ -1502,26 +2515,98 @@
       <c r="Y25">
         <v>2.2760400000000001</v>
       </c>
-      <c r="AI25">
+      <c r="AI25" s="5">
         <v>5.1886000000000001</v>
       </c>
       <c r="AJ25" s="5">
         <v>9.5263000000000009</v>
       </c>
-      <c r="AK25">
+      <c r="AK25" s="5">
         <v>-8.0340000000000007</v>
       </c>
-      <c r="AL25">
+      <c r="AL25" s="5">
         <v>-4.2249999999999996</v>
       </c>
-      <c r="AM25">
+      <c r="AM25" s="5">
         <v>-9.3440999999999992</v>
       </c>
-      <c r="AN25">
+      <c r="AN25" s="5">
         <v>115.9093</v>
       </c>
-    </row>
-    <row r="26" spans="2:40" x14ac:dyDescent="0.35">
+      <c r="AS25" s="3">
+        <v>0</v>
+      </c>
+      <c r="AT25" s="3">
+        <v>0</v>
+      </c>
+      <c r="AU25" s="3">
+        <v>-2.2273299999999998</v>
+      </c>
+      <c r="AV25" s="3">
+        <v>-8.9050999999999991</v>
+      </c>
+      <c r="AW25" s="3">
+        <v>-0.99787000000000003</v>
+      </c>
+      <c r="AX25" s="3">
+        <v>12.066330000000001</v>
+      </c>
+      <c r="BC25">
+        <v>0</v>
+      </c>
+      <c r="BD25">
+        <v>0</v>
+      </c>
+      <c r="BE25">
+        <v>9.4350799999999992</v>
+      </c>
+      <c r="BF25">
+        <v>-7.5599999999999999E-3</v>
+      </c>
+      <c r="BG25">
+        <v>2.5162399999999998</v>
+      </c>
+      <c r="BH25">
+        <v>-70.816659999999999</v>
+      </c>
+      <c r="BM25">
+        <v>0</v>
+      </c>
+      <c r="BN25">
+        <v>0</v>
+      </c>
+      <c r="BO25">
+        <v>11.838179999999999</v>
+      </c>
+      <c r="BP25">
+        <v>-3.2705799999999998</v>
+      </c>
+      <c r="BQ25">
+        <v>0.87565999999999999</v>
+      </c>
+      <c r="BR25">
+        <v>-75.965549999999993</v>
+      </c>
+      <c r="BW25">
+        <v>0</v>
+      </c>
+      <c r="BX25">
+        <v>0</v>
+      </c>
+      <c r="BY25">
+        <v>11.838179999999999</v>
+      </c>
+      <c r="BZ25">
+        <v>0</v>
+      </c>
+      <c r="CA25">
+        <v>0</v>
+      </c>
+      <c r="CB25">
+        <v>-67.255080000000007</v>
+      </c>
+    </row>
+    <row r="26" spans="2:83" x14ac:dyDescent="0.25">
       <c r="B26">
         <v>0</v>
       </c>
@@ -1579,23 +2664,95 @@
       <c r="AI26" s="5">
         <v>5.4817</v>
       </c>
-      <c r="AJ26">
+      <c r="AJ26" s="5">
         <v>-1.0106999999999999</v>
       </c>
-      <c r="AK26">
+      <c r="AK26" s="5">
         <v>-6.6711</v>
       </c>
-      <c r="AL26">
+      <c r="AL26" s="5">
         <v>-4.8913000000000002</v>
       </c>
       <c r="AM26" s="5">
         <v>4.4775</v>
       </c>
-      <c r="AN26">
+      <c r="AN26" s="5">
         <v>36.249299999999998</v>
       </c>
-    </row>
-    <row r="27" spans="2:40" x14ac:dyDescent="0.35">
+      <c r="AS26" s="3">
+        <v>0</v>
+      </c>
+      <c r="AT26" s="3">
+        <v>-7.0839699999999999</v>
+      </c>
+      <c r="AU26" s="3">
+        <v>-3.8037800000000002</v>
+      </c>
+      <c r="AV26" s="3">
+        <v>-0.93022000000000005</v>
+      </c>
+      <c r="AW26" s="3">
+        <v>7.82402</v>
+      </c>
+      <c r="AX26" s="3">
+        <v>-18.214089999999999</v>
+      </c>
+      <c r="BC26">
+        <v>0</v>
+      </c>
+      <c r="BD26">
+        <v>0</v>
+      </c>
+      <c r="BE26">
+        <v>0</v>
+      </c>
+      <c r="BF26">
+        <v>-9.1659500000000005</v>
+      </c>
+      <c r="BG26">
+        <v>-0.41560999999999998</v>
+      </c>
+      <c r="BH26">
+        <v>-4.7865799999999998</v>
+      </c>
+      <c r="BM26">
+        <v>0</v>
+      </c>
+      <c r="BN26">
+        <v>0</v>
+      </c>
+      <c r="BO26">
+        <v>0</v>
+      </c>
+      <c r="BP26">
+        <v>10.12588</v>
+      </c>
+      <c r="BQ26">
+        <v>1.65568</v>
+      </c>
+      <c r="BR26">
+        <v>-2.8949099999999999</v>
+      </c>
+      <c r="BW26">
+        <v>0</v>
+      </c>
+      <c r="BX26">
+        <v>0</v>
+      </c>
+      <c r="BY26">
+        <v>0</v>
+      </c>
+      <c r="BZ26">
+        <v>1</v>
+      </c>
+      <c r="CA26">
+        <v>0</v>
+      </c>
+      <c r="CB26">
+        <v>0.83230000000000004</v>
+      </c>
+    </row>
+    <row r="27" spans="2:83" x14ac:dyDescent="0.25">
       <c r="B27">
         <v>0</v>
       </c>
@@ -1650,26 +2807,98 @@
       <c r="Y27">
         <v>-43.49868</v>
       </c>
-      <c r="AI27">
+      <c r="AI27" s="5">
         <v>-2.5373000000000001</v>
       </c>
       <c r="AJ27" s="5">
         <v>2.5573000000000001</v>
       </c>
-      <c r="AK27">
+      <c r="AK27" s="5">
         <v>-6.9600999999999997</v>
       </c>
       <c r="AL27" s="5">
         <v>9.6417000000000002</v>
       </c>
-      <c r="AM27">
+      <c r="AM27" s="5">
         <v>-2.7947000000000002</v>
       </c>
-      <c r="AN27">
+      <c r="AN27" s="5">
         <v>47.121200000000002</v>
       </c>
-    </row>
-    <row r="28" spans="2:40" x14ac:dyDescent="0.35">
+      <c r="AS27" s="3">
+        <v>0</v>
+      </c>
+      <c r="AT27" s="3">
+        <v>4.5712299999999999</v>
+      </c>
+      <c r="AU27" s="3">
+        <v>-8.3215000000000003</v>
+      </c>
+      <c r="AV27" s="3">
+        <v>7.4531099999999997</v>
+      </c>
+      <c r="AW27" s="3">
+        <v>-3.5191300000000001</v>
+      </c>
+      <c r="AX27" s="3">
+        <v>68.217169999999996</v>
+      </c>
+      <c r="BC27">
+        <v>0</v>
+      </c>
+      <c r="BD27">
+        <v>0</v>
+      </c>
+      <c r="BE27">
+        <v>-7.1499499999999996</v>
+      </c>
+      <c r="BF27">
+        <v>5.4051200000000001</v>
+      </c>
+      <c r="BG27">
+        <v>1.8706</v>
+      </c>
+      <c r="BH27">
+        <v>32.326540000000001</v>
+      </c>
+      <c r="BM27">
+        <v>0</v>
+      </c>
+      <c r="BN27">
+        <v>0</v>
+      </c>
+      <c r="BO27">
+        <v>0</v>
+      </c>
+      <c r="BP27">
+        <v>0</v>
+      </c>
+      <c r="BQ27">
+        <v>-2.5485899999999999</v>
+      </c>
+      <c r="BR27">
+        <v>17.429010000000002</v>
+      </c>
+      <c r="BW27">
+        <v>0</v>
+      </c>
+      <c r="BX27">
+        <v>0</v>
+      </c>
+      <c r="BY27">
+        <v>0</v>
+      </c>
+      <c r="BZ27">
+        <v>0</v>
+      </c>
+      <c r="CA27">
+        <v>1</v>
+      </c>
+      <c r="CB27">
+        <v>-6.8386899999999997</v>
+      </c>
+    </row>
+    <row r="28" spans="2:83" x14ac:dyDescent="0.25">
       <c r="B28">
         <v>0</v>
       </c>
@@ -1725,24 +2954,74 @@
         <v>7.8090299999999999</v>
       </c>
     </row>
-    <row r="29" spans="2:40" x14ac:dyDescent="0.35">
-      <c r="AI29">
-        <v>1</v>
-      </c>
-      <c r="AJ29">
-        <v>0</v>
-      </c>
-      <c r="AK29">
-        <v>0</v>
-      </c>
-      <c r="AL29">
-        <v>0</v>
-      </c>
-      <c r="AM29">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="2:40" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:83" x14ac:dyDescent="0.25">
+      <c r="AI29" s="3">
+        <f>AI23/AP23</f>
+        <v>0.72321870276639511</v>
+      </c>
+      <c r="AJ29" s="3">
+        <v>0</v>
+      </c>
+      <c r="AK29" s="3">
+        <f>AI25/AP23</f>
+        <v>0.69061907587967242</v>
+      </c>
+      <c r="AL29" s="3">
+        <v>0</v>
+      </c>
+      <c r="AM29" s="3">
+        <v>0</v>
+      </c>
+      <c r="AS29" s="3">
+        <v>1</v>
+      </c>
+      <c r="AT29" s="3">
+        <v>0</v>
+      </c>
+      <c r="AU29" s="3">
+        <v>0</v>
+      </c>
+      <c r="AV29" s="3">
+        <v>0</v>
+      </c>
+      <c r="AW29" s="3">
+        <v>0</v>
+      </c>
+      <c r="BC29" s="3">
+        <v>1</v>
+      </c>
+      <c r="BD29" s="3">
+        <v>0</v>
+      </c>
+      <c r="BE29" s="3">
+        <v>0</v>
+      </c>
+      <c r="BF29" s="3">
+        <v>0</v>
+      </c>
+      <c r="BG29" s="3">
+        <v>0</v>
+      </c>
+      <c r="BW29">
+        <v>9.6401199999999996</v>
+      </c>
+      <c r="BX29">
+        <v>7.0392799999999998</v>
+      </c>
+      <c r="BY29">
+        <v>0</v>
+      </c>
+      <c r="BZ29">
+        <v>0</v>
+      </c>
+      <c r="CA29">
+        <v>0</v>
+      </c>
+      <c r="CB29">
+        <v>40.11327</v>
+      </c>
+    </row>
+    <row r="30" spans="2:83" x14ac:dyDescent="0.25">
       <c r="B30">
         <v>1</v>
       </c>
@@ -1797,23 +3076,73 @@
       <c r="Y30">
         <v>5.3648800000000003</v>
       </c>
-      <c r="AI30">
-        <v>0</v>
-      </c>
-      <c r="AJ30">
-        <v>1</v>
-      </c>
-      <c r="AK30">
-        <v>0</v>
-      </c>
-      <c r="AL30">
-        <v>0</v>
-      </c>
-      <c r="AM30">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="2:40" x14ac:dyDescent="0.35">
+      <c r="AI30" s="3">
+        <v>0</v>
+      </c>
+      <c r="AJ30" s="3">
+        <v>1</v>
+      </c>
+      <c r="AK30" s="3">
+        <v>0</v>
+      </c>
+      <c r="AL30" s="3">
+        <v>0</v>
+      </c>
+      <c r="AM30" s="3">
+        <v>0</v>
+      </c>
+      <c r="AS30" s="3">
+        <v>0</v>
+      </c>
+      <c r="AT30" s="3">
+        <f>AT24/AZ23</f>
+        <v>0.42112435989892671</v>
+      </c>
+      <c r="AU30" s="3">
+        <v>0</v>
+      </c>
+      <c r="AV30" s="3">
+        <f>AT26/AZ23</f>
+        <v>-0.90700290710654241</v>
+      </c>
+      <c r="AW30" s="3">
+        <v>0</v>
+      </c>
+      <c r="BC30" s="3">
+        <v>0</v>
+      </c>
+      <c r="BD30" s="3">
+        <v>1</v>
+      </c>
+      <c r="BE30" s="3">
+        <v>0</v>
+      </c>
+      <c r="BF30" s="3">
+        <v>0</v>
+      </c>
+      <c r="BG30" s="3">
+        <v>0</v>
+      </c>
+      <c r="BW30">
+        <v>0</v>
+      </c>
+      <c r="BX30">
+        <v>9.0496999999999996</v>
+      </c>
+      <c r="BY30">
+        <v>0</v>
+      </c>
+      <c r="BZ30">
+        <v>0</v>
+      </c>
+      <c r="CA30">
+        <v>0</v>
+      </c>
+      <c r="CB30">
+        <v>-18.467559999999999</v>
+      </c>
+    </row>
+    <row r="31" spans="2:83" x14ac:dyDescent="0.25">
       <c r="B31">
         <v>0</v>
       </c>
@@ -1868,23 +3197,75 @@
       <c r="Y31">
         <v>0.78046000000000004</v>
       </c>
-      <c r="AI31">
-        <v>0</v>
-      </c>
-      <c r="AJ31">
-        <v>0</v>
-      </c>
-      <c r="AK31">
-        <v>1</v>
-      </c>
-      <c r="AL31">
-        <v>0</v>
-      </c>
-      <c r="AM31">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="2:40" x14ac:dyDescent="0.35">
+      <c r="AI31" s="3">
+        <f>-AI25/AP23</f>
+        <v>-0.69061907587967242</v>
+      </c>
+      <c r="AJ31" s="3">
+        <v>0</v>
+      </c>
+      <c r="AK31" s="3">
+        <f>AI23/AP23</f>
+        <v>0.72321870276639511</v>
+      </c>
+      <c r="AL31" s="3">
+        <v>0</v>
+      </c>
+      <c r="AM31" s="3">
+        <v>0</v>
+      </c>
+      <c r="AS31" s="3">
+        <v>0</v>
+      </c>
+      <c r="AT31" s="3">
+        <v>0</v>
+      </c>
+      <c r="AU31" s="3">
+        <v>1</v>
+      </c>
+      <c r="AV31" s="3">
+        <v>0</v>
+      </c>
+      <c r="AW31" s="3">
+        <v>0</v>
+      </c>
+      <c r="BC31" s="3">
+        <v>0</v>
+      </c>
+      <c r="BD31" s="3">
+        <v>0</v>
+      </c>
+      <c r="BE31" s="3">
+        <f>BE25/BJ23</f>
+        <v>0.79700422972195106</v>
+      </c>
+      <c r="BF31" s="3">
+        <v>0</v>
+      </c>
+      <c r="BG31" s="3">
+        <f>BE27/BJ23</f>
+        <v>-0.60397372277717454</v>
+      </c>
+      <c r="BW31">
+        <v>0</v>
+      </c>
+      <c r="BX31">
+        <v>0</v>
+      </c>
+      <c r="BY31">
+        <v>1</v>
+      </c>
+      <c r="BZ31">
+        <v>0</v>
+      </c>
+      <c r="CA31">
+        <v>0</v>
+      </c>
+      <c r="CB31">
+        <v>-5.6811999999999996</v>
+      </c>
+    </row>
+    <row r="32" spans="2:83" x14ac:dyDescent="0.25">
       <c r="B32">
         <v>0</v>
       </c>
@@ -1939,23 +3320,73 @@
       <c r="Y32">
         <v>-0.91586000000000001</v>
       </c>
-      <c r="AI32">
-        <v>0</v>
-      </c>
-      <c r="AJ32">
-        <v>0</v>
-      </c>
-      <c r="AK32">
-        <v>0</v>
-      </c>
-      <c r="AL32">
-        <v>1</v>
-      </c>
-      <c r="AM32">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="2:39" x14ac:dyDescent="0.35">
+      <c r="AI32" s="3">
+        <v>0</v>
+      </c>
+      <c r="AJ32" s="3">
+        <v>0</v>
+      </c>
+      <c r="AK32" s="3">
+        <v>0</v>
+      </c>
+      <c r="AL32" s="3">
+        <v>1</v>
+      </c>
+      <c r="AM32" s="3">
+        <v>0</v>
+      </c>
+      <c r="AS32" s="3">
+        <v>0</v>
+      </c>
+      <c r="AT32" s="3">
+        <f>-AT26/AZ23</f>
+        <v>0.90700290710654241</v>
+      </c>
+      <c r="AU32" s="3">
+        <v>0</v>
+      </c>
+      <c r="AV32" s="3">
+        <f>AT24/AZ23</f>
+        <v>0.42112435989892671</v>
+      </c>
+      <c r="AW32" s="3">
+        <v>0</v>
+      </c>
+      <c r="BC32" s="3">
+        <v>0</v>
+      </c>
+      <c r="BD32" s="3">
+        <v>0</v>
+      </c>
+      <c r="BE32" s="3">
+        <v>0</v>
+      </c>
+      <c r="BF32" s="3">
+        <v>1</v>
+      </c>
+      <c r="BG32" s="3">
+        <v>0</v>
+      </c>
+      <c r="BW32">
+        <v>0</v>
+      </c>
+      <c r="BX32">
+        <v>0</v>
+      </c>
+      <c r="BY32">
+        <v>0</v>
+      </c>
+      <c r="BZ32">
+        <v>1</v>
+      </c>
+      <c r="CA32">
+        <v>0</v>
+      </c>
+      <c r="CB32">
+        <v>0.83230000000000004</v>
+      </c>
+    </row>
+    <row r="33" spans="2:80" x14ac:dyDescent="0.25">
       <c r="B33">
         <v>0</v>
       </c>
@@ -2010,23 +3441,73 @@
       <c r="Y33">
         <v>-6.8188399999999998</v>
       </c>
-      <c r="AI33">
-        <v>0</v>
-      </c>
-      <c r="AJ33">
-        <v>0</v>
-      </c>
-      <c r="AK33">
-        <v>0</v>
-      </c>
-      <c r="AL33">
-        <v>0</v>
-      </c>
-      <c r="AM33">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="2:39" x14ac:dyDescent="0.35">
+      <c r="AI33" s="3">
+        <v>0</v>
+      </c>
+      <c r="AJ33" s="3">
+        <v>0</v>
+      </c>
+      <c r="AK33" s="3">
+        <v>0</v>
+      </c>
+      <c r="AL33" s="3">
+        <v>0</v>
+      </c>
+      <c r="AM33" s="3">
+        <v>1</v>
+      </c>
+      <c r="AS33" s="3">
+        <v>0</v>
+      </c>
+      <c r="AT33" s="3">
+        <v>0</v>
+      </c>
+      <c r="AU33" s="3">
+        <v>0</v>
+      </c>
+      <c r="AV33" s="3">
+        <v>0</v>
+      </c>
+      <c r="AW33" s="3">
+        <v>1</v>
+      </c>
+      <c r="BC33" s="3">
+        <v>0</v>
+      </c>
+      <c r="BD33" s="3">
+        <v>0</v>
+      </c>
+      <c r="BE33" s="3">
+        <f>-BE27/BJ23</f>
+        <v>0.60397372277717454</v>
+      </c>
+      <c r="BF33" s="3">
+        <v>0</v>
+      </c>
+      <c r="BG33" s="3">
+        <f>BE25/BJ23</f>
+        <v>0.79700422972195106</v>
+      </c>
+      <c r="BW33">
+        <v>0</v>
+      </c>
+      <c r="BX33">
+        <v>0</v>
+      </c>
+      <c r="BY33">
+        <v>0</v>
+      </c>
+      <c r="BZ33">
+        <v>0</v>
+      </c>
+      <c r="CA33">
+        <v>1</v>
+      </c>
+      <c r="CB33">
+        <v>-6.8386899999999997</v>
+      </c>
+    </row>
+    <row r="34" spans="2:80" x14ac:dyDescent="0.25">
       <c r="B34">
         <v>0</v>
       </c>
@@ -2082,7 +3563,89 @@
         <v>3.4025799999999999</v>
       </c>
     </row>
-    <row r="36" spans="2:39" x14ac:dyDescent="0.35">
+    <row r="35" spans="2:80" x14ac:dyDescent="0.25">
+      <c r="AI35" s="3">
+        <v>7.5129799999999998</v>
+      </c>
+      <c r="AJ35" s="3">
+        <v>10.63339</v>
+      </c>
+      <c r="AK35" s="3">
+        <v>-2.6896599999999999</v>
+      </c>
+      <c r="AL35" s="3">
+        <v>-5.1255899999999999</v>
+      </c>
+      <c r="AM35" s="3">
+        <v>-7.1375000000000002</v>
+      </c>
+      <c r="AN35" s="3">
+        <v>80.583569999999995</v>
+      </c>
+      <c r="AP35">
+        <f>SQRT(AI35^2 + AI38^2)</f>
+        <v>9.3002098562559326</v>
+      </c>
+      <c r="AS35" s="3">
+        <v>9.6401199999999996</v>
+      </c>
+      <c r="AT35" s="3">
+        <v>7.0392799999999998</v>
+      </c>
+      <c r="AU35" s="3">
+        <v>-4.05769</v>
+      </c>
+      <c r="AV35" s="3">
+        <v>-9.3136899999999994</v>
+      </c>
+      <c r="AW35" s="3">
+        <v>-2.2809400000000002</v>
+      </c>
+      <c r="AX35" s="3">
+        <v>71.012680000000003</v>
+      </c>
+      <c r="AZ35">
+        <f>SQRT(AT36^2 + AT39^2)</f>
+        <v>9.0497008795318763</v>
+      </c>
+      <c r="BC35">
+        <v>9.6401199999999996</v>
+      </c>
+      <c r="BD35">
+        <v>7.0392799999999998</v>
+      </c>
+      <c r="BE35">
+        <v>-4.05769</v>
+      </c>
+      <c r="BF35">
+        <v>-9.3136899999999994</v>
+      </c>
+      <c r="BG35">
+        <v>-2.2809400000000002</v>
+      </c>
+      <c r="BH35">
+        <v>71.012680000000003</v>
+      </c>
+      <c r="BW35">
+        <v>9.6401199999999996</v>
+      </c>
+      <c r="BX35">
+        <v>0</v>
+      </c>
+      <c r="BY35">
+        <v>0</v>
+      </c>
+      <c r="BZ35">
+        <v>0</v>
+      </c>
+      <c r="CA35">
+        <v>0</v>
+      </c>
+      <c r="CB35">
+        <v>54.478189999999998</v>
+      </c>
+    </row>
+    <row r="36" spans="2:80" x14ac:dyDescent="0.25">
       <c r="B36">
         <v>1</v>
       </c>
@@ -2137,8 +3700,80 @@
       <c r="Y36">
         <v>1.97356</v>
       </c>
-    </row>
-    <row r="37" spans="2:39" x14ac:dyDescent="0.35">
+      <c r="AI36" s="3">
+        <v>0</v>
+      </c>
+      <c r="AJ36" s="3">
+        <v>1.3075699999999999</v>
+      </c>
+      <c r="AK36" s="3">
+        <v>-1.2726999999999999</v>
+      </c>
+      <c r="AL36" s="3">
+        <v>9.2944899999999997</v>
+      </c>
+      <c r="AM36" s="3">
+        <v>-1.55725</v>
+      </c>
+      <c r="AN36" s="3">
+        <v>22.947469999999999</v>
+      </c>
+      <c r="AS36" s="3">
+        <v>0</v>
+      </c>
+      <c r="AT36" s="3">
+        <v>7.8103100000000003</v>
+      </c>
+      <c r="AU36" s="3">
+        <v>-6.3130000000000006E-2</v>
+      </c>
+      <c r="AV36" s="3">
+        <v>2.0336699999999999</v>
+      </c>
+      <c r="AW36" s="3">
+        <v>-9.7159600000000008</v>
+      </c>
+      <c r="AX36" s="3">
+        <v>52.557319999999997</v>
+      </c>
+      <c r="BC36">
+        <v>0</v>
+      </c>
+      <c r="BD36">
+        <v>9.0496999999999996</v>
+      </c>
+      <c r="BE36">
+        <v>-4.2578800000000001</v>
+      </c>
+      <c r="BF36">
+        <v>5.5198999999999998</v>
+      </c>
+      <c r="BG36">
+        <v>-10.16292</v>
+      </c>
+      <c r="BH36">
+        <v>79.817580000000007</v>
+      </c>
+      <c r="BW36">
+        <v>0</v>
+      </c>
+      <c r="BX36">
+        <v>1</v>
+      </c>
+      <c r="BY36">
+        <v>0</v>
+      </c>
+      <c r="BZ36">
+        <v>0</v>
+      </c>
+      <c r="CA36">
+        <v>0</v>
+      </c>
+      <c r="CB36">
+        <v>-2.04068</v>
+      </c>
+    </row>
+    <row r="37" spans="2:80" x14ac:dyDescent="0.25">
       <c r="B37">
         <v>0</v>
       </c>
@@ -2193,8 +3828,80 @@
       <c r="Y37">
         <v>1.5305299999999999</v>
       </c>
-    </row>
-    <row r="38" spans="2:39" x14ac:dyDescent="0.35">
+      <c r="AI37" s="3">
+        <v>0</v>
+      </c>
+      <c r="AJ37" s="3">
+        <v>3.01803</v>
+      </c>
+      <c r="AK37" s="3">
+        <v>-8.5402699999999996</v>
+      </c>
+      <c r="AL37" s="3">
+        <v>-0.94740000000000002</v>
+      </c>
+      <c r="AM37" s="3">
+        <v>-6.1044</v>
+      </c>
+      <c r="AN37" s="3">
+        <v>83.317719999999994</v>
+      </c>
+      <c r="AS37" s="3">
+        <v>0</v>
+      </c>
+      <c r="AT37" s="3">
+        <v>0</v>
+      </c>
+      <c r="AU37" s="3">
+        <v>-2.2273299999999998</v>
+      </c>
+      <c r="AV37" s="3">
+        <v>-8.9050999999999991</v>
+      </c>
+      <c r="AW37" s="3">
+        <v>-0.99787000000000003</v>
+      </c>
+      <c r="AX37" s="3">
+        <v>12.066330000000001</v>
+      </c>
+      <c r="BC37">
+        <v>0</v>
+      </c>
+      <c r="BD37">
+        <v>0</v>
+      </c>
+      <c r="BE37">
+        <v>11.838179999999999</v>
+      </c>
+      <c r="BF37">
+        <v>-3.2705799999999998</v>
+      </c>
+      <c r="BG37">
+        <v>0.87565999999999999</v>
+      </c>
+      <c r="BH37">
+        <v>-75.965549999999993</v>
+      </c>
+      <c r="BW37">
+        <v>0</v>
+      </c>
+      <c r="BX37">
+        <v>0</v>
+      </c>
+      <c r="BY37">
+        <v>1</v>
+      </c>
+      <c r="BZ37">
+        <v>0</v>
+      </c>
+      <c r="CA37">
+        <v>0</v>
+      </c>
+      <c r="CB37">
+        <v>-5.6811999999999996</v>
+      </c>
+    </row>
+    <row r="38" spans="2:80" x14ac:dyDescent="0.25">
       <c r="B38">
         <v>0</v>
       </c>
@@ -2249,8 +3956,80 @@
       <c r="Y38">
         <v>-3.3205800000000001</v>
       </c>
-    </row>
-    <row r="39" spans="2:39" x14ac:dyDescent="0.35">
+      <c r="AI38" s="3">
+        <v>5.4817</v>
+      </c>
+      <c r="AJ38" s="3">
+        <v>-1.0106999999999999</v>
+      </c>
+      <c r="AK38" s="3">
+        <v>-6.6711</v>
+      </c>
+      <c r="AL38" s="3">
+        <v>-4.8913000000000002</v>
+      </c>
+      <c r="AM38" s="3">
+        <v>4.4775</v>
+      </c>
+      <c r="AN38" s="3">
+        <v>36.249299999999998</v>
+      </c>
+      <c r="AS38" s="3">
+        <v>0</v>
+      </c>
+      <c r="AT38" s="3">
+        <v>0</v>
+      </c>
+      <c r="AU38" s="3">
+        <v>-9.1684099999999997</v>
+      </c>
+      <c r="AV38" s="3">
+        <v>2.1711399999999998</v>
+      </c>
+      <c r="AW38" s="3">
+        <v>-2.34701</v>
+      </c>
+      <c r="AX38" s="3">
+        <v>69.945099999999996</v>
+      </c>
+      <c r="BC38">
+        <v>0</v>
+      </c>
+      <c r="BD38">
+        <v>0</v>
+      </c>
+      <c r="BE38">
+        <v>0</v>
+      </c>
+      <c r="BF38">
+        <v>-9.1659500000000005</v>
+      </c>
+      <c r="BG38">
+        <v>-0.41560999999999998</v>
+      </c>
+      <c r="BH38">
+        <v>-4.7865799999999998</v>
+      </c>
+      <c r="BW38">
+        <v>0</v>
+      </c>
+      <c r="BX38">
+        <v>0</v>
+      </c>
+      <c r="BY38">
+        <v>0</v>
+      </c>
+      <c r="BZ38">
+        <v>1</v>
+      </c>
+      <c r="CA38">
+        <v>0</v>
+      </c>
+      <c r="CB38">
+        <v>0.83230000000000004</v>
+      </c>
+    </row>
+    <row r="39" spans="2:80" x14ac:dyDescent="0.25">
       <c r="B39">
         <v>0</v>
       </c>
@@ -2305,8 +4084,80 @@
       <c r="Y39">
         <v>-4.8253000000000004</v>
       </c>
-    </row>
-    <row r="40" spans="2:39" x14ac:dyDescent="0.35">
+      <c r="AI39" s="3">
+        <v>-2.5373000000000001</v>
+      </c>
+      <c r="AJ39" s="3">
+        <v>2.5573000000000001</v>
+      </c>
+      <c r="AK39" s="3">
+        <v>-6.9600999999999997</v>
+      </c>
+      <c r="AL39" s="3">
+        <v>9.6417000000000002</v>
+      </c>
+      <c r="AM39" s="3">
+        <v>-2.7947000000000002</v>
+      </c>
+      <c r="AN39" s="3">
+        <v>47.121200000000002</v>
+      </c>
+      <c r="AS39" s="3">
+        <v>0</v>
+      </c>
+      <c r="AT39" s="3">
+        <v>4.5712299999999999</v>
+      </c>
+      <c r="AU39" s="3">
+        <v>-8.3215000000000003</v>
+      </c>
+      <c r="AV39" s="3">
+        <v>7.4531099999999997</v>
+      </c>
+      <c r="AW39" s="3">
+        <v>-3.5191300000000001</v>
+      </c>
+      <c r="AX39" s="3">
+        <v>68.217169999999996</v>
+      </c>
+      <c r="BC39">
+        <v>0</v>
+      </c>
+      <c r="BD39">
+        <v>0</v>
+      </c>
+      <c r="BE39">
+        <v>0</v>
+      </c>
+      <c r="BF39">
+        <v>4.3033400000000004</v>
+      </c>
+      <c r="BG39">
+        <v>3.0106199999999999</v>
+      </c>
+      <c r="BH39">
+        <v>-17.00704</v>
+      </c>
+      <c r="BW39">
+        <v>0</v>
+      </c>
+      <c r="BX39">
+        <v>0</v>
+      </c>
+      <c r="BY39">
+        <v>0</v>
+      </c>
+      <c r="BZ39">
+        <v>0</v>
+      </c>
+      <c r="CA39">
+        <v>1</v>
+      </c>
+      <c r="CB39">
+        <v>-6.8386899999999997</v>
+      </c>
+    </row>
+    <row r="40" spans="2:80" x14ac:dyDescent="0.25">
       <c r="B40">
         <v>0</v>
       </c>
@@ -2362,17 +4213,69 @@
         <v>2.4700899999999999</v>
       </c>
     </row>
-    <row r="42" spans="2:39" x14ac:dyDescent="0.35">
-      <c r="F42" s="3" t="s">
+    <row r="41" spans="2:80" x14ac:dyDescent="0.25">
+      <c r="AI41" s="3">
+        <f>AI35/AP35</f>
+        <v>0.8078290830121726</v>
+      </c>
+      <c r="AJ41" s="3">
+        <v>0</v>
+      </c>
+      <c r="AK41" s="3">
+        <v>0</v>
+      </c>
+      <c r="AL41" s="3">
+        <f>AI38/AP35</f>
+        <v>0.58941680722533896</v>
+      </c>
+      <c r="AM41" s="3">
+        <v>0</v>
+      </c>
+      <c r="AS41" s="3">
+        <v>1</v>
+      </c>
+      <c r="AT41" s="3">
+        <v>0</v>
+      </c>
+      <c r="AU41" s="3">
+        <v>0</v>
+      </c>
+      <c r="AV41" s="3">
+        <v>0</v>
+      </c>
+      <c r="AW41" s="3">
+        <v>0</v>
+      </c>
+      <c r="BW41">
+        <v>1</v>
+      </c>
+      <c r="BX41">
+        <v>0</v>
+      </c>
+      <c r="BY41">
+        <v>0</v>
+      </c>
+      <c r="BZ41">
+        <v>0</v>
+      </c>
+      <c r="CA41">
+        <v>0</v>
+      </c>
+      <c r="CB41">
+        <v>5.6511899999999997</v>
+      </c>
+    </row>
+    <row r="42" spans="2:80" x14ac:dyDescent="0.25">
+      <c r="F42" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="G42" s="3"/>
-      <c r="H42" s="3"/>
-      <c r="I42" s="3" t="s">
+      <c r="G42" s="4"/>
+      <c r="H42" s="4"/>
+      <c r="I42" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="J42" s="3"/>
-      <c r="K42" s="3"/>
+      <c r="J42" s="4"/>
+      <c r="K42" s="4"/>
       <c r="T42">
         <v>0</v>
       </c>
@@ -2391,8 +4294,58 @@
       <c r="Y42">
         <v>-2.0405899999999999</v>
       </c>
-    </row>
-    <row r="43" spans="2:39" x14ac:dyDescent="0.35">
+      <c r="AI42" s="3">
+        <v>0</v>
+      </c>
+      <c r="AJ42" s="3">
+        <v>1</v>
+      </c>
+      <c r="AK42" s="3">
+        <v>0</v>
+      </c>
+      <c r="AL42" s="3">
+        <v>0</v>
+      </c>
+      <c r="AM42" s="3">
+        <v>0</v>
+      </c>
+      <c r="AS42" s="3">
+        <v>0</v>
+      </c>
+      <c r="AT42" s="3">
+        <f>AT36/AZ35</f>
+        <v>0.86304620494860074</v>
+      </c>
+      <c r="AU42" s="3">
+        <v>0</v>
+      </c>
+      <c r="AV42" s="3">
+        <v>0</v>
+      </c>
+      <c r="AW42" s="3">
+        <f>AT39/AZ35</f>
+        <v>0.50512498267638439</v>
+      </c>
+      <c r="BW42">
+        <v>0</v>
+      </c>
+      <c r="BX42">
+        <v>1</v>
+      </c>
+      <c r="BY42">
+        <v>0</v>
+      </c>
+      <c r="BZ42">
+        <v>0</v>
+      </c>
+      <c r="CA42">
+        <v>0</v>
+      </c>
+      <c r="CB42">
+        <v>-2.04068</v>
+      </c>
+    </row>
+    <row r="43" spans="2:80" x14ac:dyDescent="0.25">
       <c r="G43" t="s">
         <v>7</v>
       </c>
@@ -2425,10 +4378,58 @@
       <c r="Y43">
         <v>0.83223000000000003</v>
       </c>
-    </row>
-    <row r="44" spans="2:39" x14ac:dyDescent="0.35">
+      <c r="AI43" s="3">
+        <v>0</v>
+      </c>
+      <c r="AJ43" s="3">
+        <v>0</v>
+      </c>
+      <c r="AK43" s="3">
+        <v>1</v>
+      </c>
+      <c r="AL43" s="3">
+        <v>0</v>
+      </c>
+      <c r="AM43" s="3">
+        <v>0</v>
+      </c>
+      <c r="AS43" s="3">
+        <v>0</v>
+      </c>
+      <c r="AT43" s="3">
+        <v>0</v>
+      </c>
+      <c r="AU43" s="3">
+        <v>1</v>
+      </c>
+      <c r="AV43" s="3">
+        <v>0</v>
+      </c>
+      <c r="AW43" s="3">
+        <v>0</v>
+      </c>
+      <c r="BW43">
+        <v>0</v>
+      </c>
+      <c r="BX43">
+        <v>0</v>
+      </c>
+      <c r="BY43">
+        <v>1</v>
+      </c>
+      <c r="BZ43">
+        <v>0</v>
+      </c>
+      <c r="CA43">
+        <v>0</v>
+      </c>
+      <c r="CB43">
+        <v>-5.6811999999999996</v>
+      </c>
+    </row>
+    <row r="44" spans="2:80" x14ac:dyDescent="0.25">
       <c r="H44">
-        <f t="shared" ref="H44:H47" si="1">G13 - B13 * $O$36 - C13 * $O$37 - D13*$O$38 - E13*$O$39 - F13*$O$40</f>
+        <f t="shared" ref="H44:H47" si="2">G13 - B13 * $O$36 - C13 * $O$37 - D13*$O$38 - E13*$O$39 - F13*$O$40</f>
         <v>5.455299999468366E-5</v>
       </c>
       <c r="T44">
@@ -2449,10 +4450,60 @@
       <c r="Y44">
         <v>-6.83866</v>
       </c>
-    </row>
-    <row r="45" spans="2:39" x14ac:dyDescent="0.35">
+      <c r="AI44" s="3">
+        <f>-AI38/AP35</f>
+        <v>-0.58941680722533896</v>
+      </c>
+      <c r="AJ44" s="3">
+        <v>0</v>
+      </c>
+      <c r="AK44" s="3">
+        <v>0</v>
+      </c>
+      <c r="AL44" s="3">
+        <f>AI35/AP35</f>
+        <v>0.8078290830121726</v>
+      </c>
+      <c r="AM44" s="3">
+        <v>0</v>
+      </c>
+      <c r="AS44" s="3">
+        <v>0</v>
+      </c>
+      <c r="AT44" s="3">
+        <v>0</v>
+      </c>
+      <c r="AU44" s="3">
+        <v>0</v>
+      </c>
+      <c r="AV44" s="3">
+        <v>1</v>
+      </c>
+      <c r="AW44" s="3">
+        <v>0</v>
+      </c>
+      <c r="BW44">
+        <v>0</v>
+      </c>
+      <c r="BX44">
+        <v>0</v>
+      </c>
+      <c r="BY44">
+        <v>0</v>
+      </c>
+      <c r="BZ44">
+        <v>1</v>
+      </c>
+      <c r="CA44">
+        <v>0</v>
+      </c>
+      <c r="CB44">
+        <v>0.83230000000000004</v>
+      </c>
+    </row>
+    <row r="45" spans="2:80" x14ac:dyDescent="0.25">
       <c r="H45">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-7.0419000000043752E-4</v>
       </c>
       <c r="T45">
@@ -2473,10 +4524,60 @@
       <c r="Y45">
         <v>-5.6811600000000002</v>
       </c>
-    </row>
-    <row r="46" spans="2:39" x14ac:dyDescent="0.35">
+      <c r="AI45" s="3">
+        <v>0</v>
+      </c>
+      <c r="AJ45" s="3">
+        <v>0</v>
+      </c>
+      <c r="AK45" s="3">
+        <v>0</v>
+      </c>
+      <c r="AL45" s="3">
+        <v>0</v>
+      </c>
+      <c r="AM45" s="3">
+        <v>1</v>
+      </c>
+      <c r="AS45" s="3">
+        <v>0</v>
+      </c>
+      <c r="AT45" s="3">
+        <f>-AT39/AZ35</f>
+        <v>-0.50512498267638439</v>
+      </c>
+      <c r="AU45" s="3">
+        <v>0</v>
+      </c>
+      <c r="AV45" s="3">
+        <v>0</v>
+      </c>
+      <c r="AW45" s="3">
+        <f>AT36/AZ35</f>
+        <v>0.86304620494860074</v>
+      </c>
+      <c r="BW45">
+        <v>0</v>
+      </c>
+      <c r="BX45">
+        <v>0</v>
+      </c>
+      <c r="BY45">
+        <v>0</v>
+      </c>
+      <c r="BZ45">
+        <v>0</v>
+      </c>
+      <c r="CA45">
+        <v>1</v>
+      </c>
+      <c r="CB45">
+        <v>-6.8386899999999997</v>
+      </c>
+    </row>
+    <row r="46" spans="2:80" x14ac:dyDescent="0.25">
       <c r="H46">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2.3615819999953658E-3</v>
       </c>
       <c r="T46">
@@ -2498,13 +4599,53 @@
         <v>5.6511500000000003</v>
       </c>
     </row>
-    <row r="47" spans="2:39" x14ac:dyDescent="0.35">
+    <row r="47" spans="2:80" x14ac:dyDescent="0.25">
       <c r="H47">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.0412160000115023E-3</v>
       </c>
-    </row>
-    <row r="48" spans="2:39" x14ac:dyDescent="0.35">
+      <c r="AI47" s="3">
+        <v>9.3002099999999999</v>
+      </c>
+      <c r="AJ47" s="3">
+        <v>7.9942399999999996</v>
+      </c>
+      <c r="AK47" s="3">
+        <v>-6.1048499999999999</v>
+      </c>
+      <c r="AL47" s="3">
+        <v>-7.0236200000000002</v>
+      </c>
+      <c r="AM47" s="3">
+        <v>-3.12676</v>
+      </c>
+      <c r="AN47" s="3">
+        <v>86.463700000000003</v>
+      </c>
+      <c r="AP47">
+        <f>SQRT(AI47^2 + AI51^2)</f>
+        <v>9.6401139689372961</v>
+      </c>
+      <c r="AS47">
+        <v>9.6401199999999996</v>
+      </c>
+      <c r="AT47">
+        <v>7.0392799999999998</v>
+      </c>
+      <c r="AU47">
+        <v>-4.05769</v>
+      </c>
+      <c r="AV47">
+        <v>-9.3136899999999994</v>
+      </c>
+      <c r="AW47">
+        <v>-2.2809400000000002</v>
+      </c>
+      <c r="AX47">
+        <v>71.012680000000003</v>
+      </c>
+    </row>
+    <row r="48" spans="2:80" x14ac:dyDescent="0.25">
       <c r="T48">
         <v>1</v>
       </c>
@@ -2523,8 +4664,44 @@
       <c r="Y48">
         <v>5.6511500000000003</v>
       </c>
-    </row>
-    <row r="49" spans="20:25" x14ac:dyDescent="0.35">
+      <c r="AI48" s="3">
+        <v>0</v>
+      </c>
+      <c r="AJ48" s="3">
+        <v>1.3075699999999999</v>
+      </c>
+      <c r="AK48" s="3">
+        <v>-1.2726999999999999</v>
+      </c>
+      <c r="AL48" s="3">
+        <v>9.2944899999999997</v>
+      </c>
+      <c r="AM48" s="3">
+        <v>-1.55725</v>
+      </c>
+      <c r="AN48" s="3">
+        <v>22.947469999999999</v>
+      </c>
+      <c r="AS48">
+        <v>0</v>
+      </c>
+      <c r="AT48">
+        <v>9.0496999999999996</v>
+      </c>
+      <c r="AU48">
+        <v>-4.2578800000000001</v>
+      </c>
+      <c r="AV48">
+        <v>5.5198999999999998</v>
+      </c>
+      <c r="AW48">
+        <v>-10.16292</v>
+      </c>
+      <c r="AX48">
+        <v>79.817580000000007</v>
+      </c>
+    </row>
+    <row r="49" spans="20:50" x14ac:dyDescent="0.25">
       <c r="T49">
         <v>0</v>
       </c>
@@ -2543,8 +4720,44 @@
       <c r="Y49">
         <v>-2.0405899999999999</v>
       </c>
-    </row>
-    <row r="50" spans="20:25" x14ac:dyDescent="0.35">
+      <c r="AI49" s="3">
+        <v>0</v>
+      </c>
+      <c r="AJ49" s="3">
+        <v>3.01803</v>
+      </c>
+      <c r="AK49" s="3">
+        <v>-8.5402699999999996</v>
+      </c>
+      <c r="AL49" s="3">
+        <v>-0.94740000000000002</v>
+      </c>
+      <c r="AM49" s="3">
+        <v>-6.1044</v>
+      </c>
+      <c r="AN49" s="3">
+        <v>83.317719999999994</v>
+      </c>
+      <c r="AS49">
+        <v>0</v>
+      </c>
+      <c r="AT49">
+        <v>0</v>
+      </c>
+      <c r="AU49">
+        <v>-2.2273299999999998</v>
+      </c>
+      <c r="AV49">
+        <v>-8.9050999999999991</v>
+      </c>
+      <c r="AW49">
+        <v>-0.99787000000000003</v>
+      </c>
+      <c r="AX49">
+        <v>12.066330000000001</v>
+      </c>
+    </row>
+    <row r="50" spans="20:50" x14ac:dyDescent="0.25">
       <c r="T50">
         <v>0</v>
       </c>
@@ -2563,8 +4776,44 @@
       <c r="Y50">
         <v>-5.6811600000000002</v>
       </c>
-    </row>
-    <row r="51" spans="20:25" x14ac:dyDescent="0.35">
+      <c r="AI50" s="3">
+        <v>0</v>
+      </c>
+      <c r="AJ50" s="3">
+        <v>-7.0839699999999999</v>
+      </c>
+      <c r="AK50" s="3">
+        <v>-3.8037800000000002</v>
+      </c>
+      <c r="AL50" s="3">
+        <v>-0.93022000000000005</v>
+      </c>
+      <c r="AM50" s="3">
+        <v>7.82402</v>
+      </c>
+      <c r="AN50" s="3">
+        <v>-18.214089999999999</v>
+      </c>
+      <c r="AS50">
+        <v>0</v>
+      </c>
+      <c r="AT50">
+        <v>0</v>
+      </c>
+      <c r="AU50">
+        <v>-9.1684099999999997</v>
+      </c>
+      <c r="AV50">
+        <v>2.1711399999999998</v>
+      </c>
+      <c r="AW50">
+        <v>-2.34701</v>
+      </c>
+      <c r="AX50">
+        <v>69.945099999999996</v>
+      </c>
+    </row>
+    <row r="51" spans="20:50" x14ac:dyDescent="0.25">
       <c r="T51">
         <v>0</v>
       </c>
@@ -2583,8 +4832,44 @@
       <c r="Y51">
         <v>0.83223000000000003</v>
       </c>
-    </row>
-    <row r="52" spans="20:25" x14ac:dyDescent="0.35">
+      <c r="AI51" s="3">
+        <v>-2.5373000000000001</v>
+      </c>
+      <c r="AJ51" s="3">
+        <v>2.5573000000000001</v>
+      </c>
+      <c r="AK51" s="3">
+        <v>-6.9600999999999997</v>
+      </c>
+      <c r="AL51" s="3">
+        <v>9.6417000000000002</v>
+      </c>
+      <c r="AM51" s="3">
+        <v>-2.7947000000000002</v>
+      </c>
+      <c r="AN51" s="3">
+        <v>47.121200000000002</v>
+      </c>
+      <c r="AS51">
+        <v>0</v>
+      </c>
+      <c r="AT51">
+        <v>0</v>
+      </c>
+      <c r="AU51">
+        <v>-7.1499499999999996</v>
+      </c>
+      <c r="AV51">
+        <v>5.4051200000000001</v>
+      </c>
+      <c r="AW51">
+        <v>1.8706</v>
+      </c>
+      <c r="AX51">
+        <v>32.326540000000001</v>
+      </c>
+    </row>
+    <row r="52" spans="20:50" x14ac:dyDescent="0.25">
       <c r="T52">
         <v>0</v>
       </c>
@@ -2604,8 +4889,200 @@
         <v>-6.83866</v>
       </c>
     </row>
+    <row r="53" spans="20:50" x14ac:dyDescent="0.25">
+      <c r="AI53" s="3">
+        <f>AI47/AP47</f>
+        <v>0.96474066903850453</v>
+      </c>
+      <c r="AJ53" s="3">
+        <v>0</v>
+      </c>
+      <c r="AK53" s="3">
+        <v>0</v>
+      </c>
+      <c r="AL53" s="3">
+        <v>0</v>
+      </c>
+      <c r="AM53" s="3">
+        <f>AI51/AP47</f>
+        <v>-0.26320228248086847</v>
+      </c>
+    </row>
+    <row r="54" spans="20:50" x14ac:dyDescent="0.25">
+      <c r="AI54" s="3">
+        <v>0</v>
+      </c>
+      <c r="AJ54" s="3">
+        <v>1</v>
+      </c>
+      <c r="AK54" s="3">
+        <v>0</v>
+      </c>
+      <c r="AL54" s="3">
+        <v>0</v>
+      </c>
+      <c r="AM54" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="20:50" x14ac:dyDescent="0.25">
+      <c r="AI55" s="3">
+        <v>0</v>
+      </c>
+      <c r="AJ55" s="3">
+        <v>0</v>
+      </c>
+      <c r="AK55" s="3">
+        <v>1</v>
+      </c>
+      <c r="AL55" s="3">
+        <v>0</v>
+      </c>
+      <c r="AM55" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="20:50" x14ac:dyDescent="0.25">
+      <c r="AI56" s="3">
+        <v>0</v>
+      </c>
+      <c r="AJ56" s="3">
+        <v>0</v>
+      </c>
+      <c r="AK56" s="3">
+        <v>0</v>
+      </c>
+      <c r="AL56" s="3">
+        <v>1</v>
+      </c>
+      <c r="AM56" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="20:50" x14ac:dyDescent="0.25">
+      <c r="AI57" s="3">
+        <f>-AI51/AP47</f>
+        <v>0.26320228248086847</v>
+      </c>
+      <c r="AJ57" s="3">
+        <v>0</v>
+      </c>
+      <c r="AK57" s="3">
+        <v>0</v>
+      </c>
+      <c r="AL57" s="3">
+        <v>0</v>
+      </c>
+      <c r="AM57" s="3">
+        <f>AI47/AP47</f>
+        <v>0.96474066903850453</v>
+      </c>
+    </row>
+    <row r="59" spans="20:50" x14ac:dyDescent="0.25">
+      <c r="AI59">
+        <v>9.6401199999999996</v>
+      </c>
+      <c r="AJ59">
+        <v>7.0392799999999998</v>
+      </c>
+      <c r="AK59">
+        <v>-4.05769</v>
+      </c>
+      <c r="AL59">
+        <v>-9.3136899999999994</v>
+      </c>
+      <c r="AM59">
+        <v>-2.2809400000000002</v>
+      </c>
+      <c r="AN59">
+        <v>71.012680000000003</v>
+      </c>
+    </row>
+    <row r="60" spans="20:50" x14ac:dyDescent="0.25">
+      <c r="AI60">
+        <v>0</v>
+      </c>
+      <c r="AJ60">
+        <v>1.3075699999999999</v>
+      </c>
+      <c r="AK60">
+        <v>-1.2726999999999999</v>
+      </c>
+      <c r="AL60">
+        <v>9.2944899999999997</v>
+      </c>
+      <c r="AM60">
+        <v>-1.55725</v>
+      </c>
+      <c r="AN60">
+        <v>22.947469999999999</v>
+      </c>
+    </row>
+    <row r="61" spans="20:50" x14ac:dyDescent="0.25">
+      <c r="AI61">
+        <v>0</v>
+      </c>
+      <c r="AJ61">
+        <v>3.01803</v>
+      </c>
+      <c r="AK61">
+        <v>-8.5402699999999996</v>
+      </c>
+      <c r="AL61">
+        <v>-0.94740000000000002</v>
+      </c>
+      <c r="AM61">
+        <v>-6.1044</v>
+      </c>
+      <c r="AN61">
+        <v>83.317719999999994</v>
+      </c>
+    </row>
+    <row r="62" spans="20:50" x14ac:dyDescent="0.25">
+      <c r="AI62">
+        <v>0</v>
+      </c>
+      <c r="AJ62">
+        <v>-7.0839699999999999</v>
+      </c>
+      <c r="AK62">
+        <v>-3.8037800000000002</v>
+      </c>
+      <c r="AL62">
+        <v>-0.93022000000000005</v>
+      </c>
+      <c r="AM62">
+        <v>7.82402</v>
+      </c>
+      <c r="AN62">
+        <v>-18.214089999999999</v>
+      </c>
+    </row>
+    <row r="63" spans="20:50" x14ac:dyDescent="0.25">
+      <c r="AI63">
+        <v>0</v>
+      </c>
+      <c r="AJ63">
+        <v>4.5712299999999999</v>
+      </c>
+      <c r="AK63">
+        <v>-8.3215000000000003</v>
+      </c>
+      <c r="AL63">
+        <v>7.4531099999999997</v>
+      </c>
+      <c r="AM63">
+        <v>-3.5191300000000001</v>
+      </c>
+      <c r="AN63">
+        <v>68.217169999999996</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="13">
+    <mergeCell ref="BW3:CB3"/>
+    <mergeCell ref="CD11:CE11"/>
+    <mergeCell ref="CD18:CE18"/>
     <mergeCell ref="F3:K3"/>
     <mergeCell ref="F42:H42"/>
     <mergeCell ref="I42:K42"/>

</xml_diff>